<commit_message>
SVI calib slice par slice
</commit_message>
<xml_diff>
--- a/data/option_data/option_data_SPX.xlsx
+++ b/data/option_data/option_data_SPX.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thibc\OneDrive\Documents\Dev\Structured-Product-Pricing-Python\data\option_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F581E810-8FFA-46A7-9F8E-FD919AE204F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Feuil1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Maturity</t>
   </si>
@@ -44,9 +50,6 @@
   </si>
   <si>
     <t>9W</t>
-  </si>
-  <si>
-    <t>10W</t>
   </si>
   <si>
     <t>11W</t>
@@ -79,8 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,35 +125,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -162,10 +164,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -203,71 +205,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -295,7 +297,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -318,11 +320,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -331,13 +333,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -347,7 +349,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -356,7 +358,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -365,7 +367,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -373,10 +375,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -441,38 +443,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="6.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="6.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="6" width="6.005" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="5" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="5" width="7.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="14" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="7" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,7 +522,7 @@
         <v>8653.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -575,7 +566,7 @@
         <v>28.26</v>
       </c>
       <c r="O2" s="2">
-        <v>32.37</v>
+        <v>32.369999999999997</v>
       </c>
       <c r="P2" s="2">
         <v>39.72</v>
@@ -590,7 +581,7 @@
         <v>68.58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -628,7 +619,7 @@
         <v>15.5</v>
       </c>
       <c r="M3" s="2">
-        <v>18.49</v>
+        <v>18.489999999999998</v>
       </c>
       <c r="N3" s="2">
         <v>21.74</v>
@@ -640,7 +631,7 @@
         <v>30.84</v>
       </c>
       <c r="Q3" s="2">
-        <v>36.09</v>
+        <v>36.090000000000003</v>
       </c>
       <c r="R3" s="2">
         <v>40.79</v>
@@ -649,21 +640,21 @@
         <v>55.56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>70.46</v>
+        <v>70.459999999999994</v>
       </c>
       <c r="C4" s="2">
-        <v>39.16</v>
+        <v>39.159999999999997</v>
       </c>
       <c r="D4" s="2">
         <v>24.77</v>
       </c>
       <c r="E4" s="2">
-        <v>19.94</v>
+        <v>19.940000000000001</v>
       </c>
       <c r="F4" s="3">
         <v>18</v>
@@ -702,13 +693,13 @@
         <v>31.2</v>
       </c>
       <c r="R4" s="2">
-        <v>35.37</v>
+        <v>35.369999999999997</v>
       </c>
       <c r="S4" s="2">
         <v>48.76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -716,7 +707,7 @@
         <v>63.01</v>
       </c>
       <c r="C5" s="2">
-        <v>34.8</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="D5" s="2">
         <v>23.36</v>
@@ -725,7 +716,7 @@
         <v>19.18</v>
       </c>
       <c r="F5" s="2">
-        <v>17.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="G5" s="2">
         <v>15.41</v>
@@ -752,7 +743,7 @@
         <v>16.11</v>
       </c>
       <c r="O5" s="2">
-        <v>18.49</v>
+        <v>18.489999999999998</v>
       </c>
       <c r="P5" s="2">
         <v>22.99</v>
@@ -767,7 +758,7 @@
         <v>42.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -781,7 +772,7 @@
         <v>22.84</v>
       </c>
       <c r="E6" s="2">
-        <v>18.81</v>
+        <v>18.809999999999999</v>
       </c>
       <c r="F6" s="2">
         <v>17.05</v>
@@ -826,7 +817,7 @@
         <v>41.09</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -840,7 +831,7 @@
         <v>22.88</v>
       </c>
       <c r="E7" s="2">
-        <v>19.08</v>
+        <v>19.079999999999998</v>
       </c>
       <c r="F7" s="2">
         <v>17.38</v>
@@ -885,7 +876,7 @@
         <v>38.57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -899,10 +890,10 @@
         <v>22.45</v>
       </c>
       <c r="E8" s="2">
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="F8" s="2">
-        <v>17.24</v>
+        <v>17.239999999999998</v>
       </c>
       <c r="G8" s="2">
         <v>15.38</v>
@@ -944,7 +935,7 @@
         <v>36.57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -958,10 +949,10 @@
         <v>22.02</v>
       </c>
       <c r="E9" s="2">
-        <v>18.76</v>
+        <v>18.760000000000002</v>
       </c>
       <c r="F9" s="2">
-        <v>17.17</v>
+        <v>17.170000000000002</v>
       </c>
       <c r="G9" s="2">
         <v>15.42</v>
@@ -991,7 +982,7 @@
         <v>14.3</v>
       </c>
       <c r="P9" s="2">
-        <v>17.83</v>
+        <v>17.829999999999998</v>
       </c>
       <c r="Q9" s="2">
         <v>21.06</v>
@@ -1003,7 +994,7 @@
         <v>33.82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1017,10 +1008,10 @@
         <v>21.97</v>
       </c>
       <c r="E10" s="2">
-        <v>18.74</v>
+        <v>18.739999999999998</v>
       </c>
       <c r="F10" s="2">
-        <v>17.17</v>
+        <v>17.170000000000002</v>
       </c>
       <c r="G10" s="2">
         <v>15.43</v>
@@ -1062,593 +1053,534 @@
         <v>33.43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>49.53</v>
+        <v>48.13</v>
       </c>
       <c r="C11" s="2">
-        <v>29.08</v>
+        <v>28.72</v>
       </c>
       <c r="D11" s="2">
-        <v>21.79</v>
+        <v>21.64</v>
       </c>
       <c r="E11" s="2">
-        <v>18.71</v>
+        <v>18.690000000000001</v>
       </c>
       <c r="F11" s="2">
-        <v>17.17</v>
+        <v>17.190000000000001</v>
       </c>
       <c r="G11" s="2">
-        <v>15.49</v>
+        <v>15.55</v>
       </c>
       <c r="H11" s="2">
-        <v>14.8</v>
+        <v>14.88</v>
       </c>
       <c r="I11" s="2">
-        <v>13.84</v>
+        <v>13.94</v>
       </c>
       <c r="J11" s="2">
-        <v>12.6</v>
+        <v>12.69</v>
       </c>
       <c r="K11" s="2">
-        <v>12.26</v>
+        <v>12.34</v>
       </c>
       <c r="L11" s="2">
-        <v>11.89</v>
+        <v>11.95</v>
       </c>
       <c r="M11" s="2">
-        <v>11.57</v>
+        <v>11.59</v>
       </c>
       <c r="N11" s="2">
-        <v>12.1</v>
+        <v>11.92</v>
       </c>
       <c r="O11" s="2">
-        <v>13.6</v>
+        <v>13.21</v>
       </c>
       <c r="P11" s="2">
-        <v>16.9</v>
+        <v>16.3</v>
       </c>
       <c r="Q11" s="2">
-        <v>19.97</v>
+        <v>19.239999999999998</v>
       </c>
       <c r="R11" s="2">
-        <v>22.79</v>
+        <v>21.97</v>
       </c>
       <c r="S11" s="2">
-        <v>32.16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+        <v>31.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>48.13</v>
+        <v>45.59</v>
       </c>
       <c r="C12" s="2">
-        <v>28.72</v>
+        <v>27.95</v>
       </c>
       <c r="D12" s="2">
-        <v>21.64</v>
+        <v>21.35</v>
       </c>
       <c r="E12" s="2">
-        <v>18.69</v>
+        <v>18.61</v>
       </c>
       <c r="F12" s="2">
-        <v>17.19</v>
+        <v>17.18</v>
       </c>
       <c r="G12" s="2">
-        <v>15.55</v>
+        <v>15.62</v>
       </c>
       <c r="H12" s="2">
-        <v>14.88</v>
+        <v>14.98</v>
       </c>
       <c r="I12" s="2">
-        <v>13.94</v>
+        <v>14.07</v>
       </c>
       <c r="J12" s="2">
-        <v>12.69</v>
+        <v>12.8</v>
       </c>
       <c r="K12" s="2">
-        <v>12.34</v>
+        <v>12.41</v>
       </c>
       <c r="L12" s="2">
-        <v>11.95</v>
+        <v>11.97</v>
       </c>
       <c r="M12" s="2">
-        <v>11.59</v>
+        <v>11.56</v>
       </c>
       <c r="N12" s="2">
-        <v>11.92</v>
+        <v>11.58</v>
       </c>
       <c r="O12" s="2">
-        <v>13.21</v>
+        <v>12.43</v>
       </c>
       <c r="P12" s="2">
-        <v>16.3</v>
+        <v>15.19</v>
       </c>
       <c r="Q12" s="2">
-        <v>19.24</v>
+        <v>17.940000000000001</v>
       </c>
       <c r="R12" s="2">
-        <v>21.97</v>
+        <v>20.49</v>
       </c>
       <c r="S12" s="2">
-        <v>31.05</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+        <v>29.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>45.59</v>
+        <v>37.51</v>
       </c>
       <c r="C13" s="2">
-        <v>27.95</v>
+        <v>25.35</v>
       </c>
       <c r="D13" s="2">
-        <v>21.35</v>
+        <v>20.7</v>
       </c>
       <c r="E13" s="2">
-        <v>18.61</v>
+        <v>18.62</v>
       </c>
       <c r="F13" s="2">
-        <v>17.18</v>
+        <v>17.52</v>
       </c>
       <c r="G13" s="2">
-        <v>15.62</v>
+        <v>16.36</v>
       </c>
       <c r="H13" s="2">
-        <v>14.98</v>
+        <v>15.88</v>
       </c>
       <c r="I13" s="2">
-        <v>14.07</v>
+        <v>15.17</v>
       </c>
       <c r="J13" s="2">
-        <v>12.8</v>
+        <v>14.03</v>
       </c>
       <c r="K13" s="2">
-        <v>12.41</v>
+        <v>13.6</v>
       </c>
       <c r="L13" s="2">
-        <v>11.97</v>
+        <v>13.02</v>
       </c>
       <c r="M13" s="2">
-        <v>11.56</v>
+        <v>12.21</v>
       </c>
       <c r="N13" s="2">
-        <v>11.58</v>
+        <v>11.63</v>
       </c>
       <c r="O13" s="2">
-        <v>12.43</v>
+        <v>11.33</v>
       </c>
       <c r="P13" s="2">
-        <v>15.19</v>
+        <v>11.76</v>
       </c>
       <c r="Q13" s="2">
-        <v>17.94</v>
+        <v>13.3</v>
       </c>
       <c r="R13" s="2">
-        <v>20.49</v>
+        <v>15.14</v>
       </c>
       <c r="S13" s="2">
-        <v>29.03</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+        <v>21.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>37.51</v>
+        <v>34.409999999999997</v>
       </c>
       <c r="C14" s="2">
-        <v>25.35</v>
+        <v>24.08</v>
       </c>
       <c r="D14" s="2">
-        <v>20.7</v>
+        <v>20.38</v>
       </c>
       <c r="E14" s="2">
-        <v>18.62</v>
+        <v>18.64</v>
       </c>
       <c r="F14" s="2">
-        <v>17.52</v>
+        <v>17.73</v>
       </c>
       <c r="G14" s="2">
-        <v>16.36</v>
+        <v>16.79</v>
       </c>
       <c r="H14" s="2">
-        <v>15.88</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="I14" s="2">
-        <v>15.17</v>
+        <v>15.81</v>
       </c>
       <c r="J14" s="2">
-        <v>14.03</v>
+        <v>14.82</v>
       </c>
       <c r="K14" s="2">
-        <v>13.6</v>
+        <v>14.44</v>
       </c>
       <c r="L14" s="2">
-        <v>13.02</v>
+        <v>13.88</v>
       </c>
       <c r="M14" s="2">
-        <v>12.21</v>
+        <v>13.03</v>
       </c>
       <c r="N14" s="2">
-        <v>11.63</v>
+        <v>12.33</v>
       </c>
       <c r="O14" s="2">
-        <v>11.33</v>
+        <v>11.8</v>
       </c>
       <c r="P14" s="2">
-        <v>11.76</v>
+        <v>11.34</v>
       </c>
       <c r="Q14" s="2">
-        <v>13.3</v>
+        <v>11.69</v>
       </c>
       <c r="R14" s="2">
-        <v>15.14</v>
+        <v>12.67</v>
       </c>
       <c r="S14" s="2">
-        <v>21.7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+        <v>17.86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>34.41</v>
+        <v>33.57</v>
       </c>
       <c r="C15" s="2">
-        <v>24.08</v>
+        <v>23.7</v>
       </c>
       <c r="D15" s="2">
-        <v>20.38</v>
+        <v>20.18</v>
       </c>
       <c r="E15" s="2">
-        <v>18.64</v>
+        <v>18.53</v>
       </c>
       <c r="F15" s="2">
-        <v>17.73</v>
+        <v>17.68</v>
       </c>
       <c r="G15" s="2">
-        <v>16.79</v>
+        <v>16.8</v>
       </c>
       <c r="H15" s="2">
-        <v>16.4</v>
+        <v>16.43</v>
       </c>
       <c r="I15" s="2">
-        <v>15.81</v>
+        <v>15.87</v>
       </c>
       <c r="J15" s="2">
-        <v>14.82</v>
+        <v>14.94</v>
       </c>
       <c r="K15" s="2">
-        <v>14.44</v>
+        <v>14.57</v>
       </c>
       <c r="L15" s="2">
-        <v>13.88</v>
+        <v>14.03</v>
       </c>
       <c r="M15" s="2">
-        <v>13.03</v>
+        <v>13.19</v>
       </c>
       <c r="N15" s="2">
-        <v>12.33</v>
+        <v>12.48</v>
       </c>
       <c r="O15" s="2">
-        <v>11.8</v>
+        <v>11.91</v>
       </c>
       <c r="P15" s="2">
-        <v>11.34</v>
+        <v>11.29</v>
       </c>
       <c r="Q15" s="2">
-        <v>11.69</v>
+        <v>11.41</v>
       </c>
       <c r="R15" s="2">
-        <v>12.67</v>
+        <v>12.17</v>
       </c>
       <c r="S15" s="2">
-        <v>17.86</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+        <v>16.89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>33.57</v>
+        <v>32.270000000000003</v>
       </c>
       <c r="C16" s="2">
-        <v>23.7</v>
+        <v>23.38</v>
       </c>
       <c r="D16" s="2">
         <v>20.18</v>
       </c>
       <c r="E16" s="2">
-        <v>18.53</v>
+        <v>18.670000000000002</v>
       </c>
       <c r="F16" s="2">
-        <v>17.68</v>
+        <v>17.89</v>
       </c>
       <c r="G16" s="2">
-        <v>16.8</v>
+        <v>17.079999999999998</v>
       </c>
       <c r="H16" s="2">
-        <v>16.43</v>
+        <v>16.75</v>
       </c>
       <c r="I16" s="2">
-        <v>15.87</v>
+        <v>16.239999999999998</v>
       </c>
       <c r="J16" s="2">
-        <v>14.94</v>
+        <v>15.38</v>
       </c>
       <c r="K16" s="2">
-        <v>14.57</v>
+        <v>15.04</v>
       </c>
       <c r="L16" s="2">
-        <v>14.03</v>
+        <v>14.54</v>
       </c>
       <c r="M16" s="2">
-        <v>13.19</v>
+        <v>13.75</v>
       </c>
       <c r="N16" s="2">
-        <v>12.48</v>
+        <v>13.04</v>
       </c>
       <c r="O16" s="2">
-        <v>11.91</v>
+        <v>12.45</v>
       </c>
       <c r="P16" s="2">
-        <v>11.29</v>
+        <v>11.64</v>
       </c>
       <c r="Q16" s="2">
-        <v>11.41</v>
+        <v>11.38</v>
       </c>
       <c r="R16" s="2">
-        <v>12.17</v>
+        <v>11.68</v>
       </c>
       <c r="S16" s="2">
-        <v>16.89</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+        <v>15.44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>32.27</v>
+        <v>29.33</v>
       </c>
       <c r="C17" s="2">
-        <v>23.38</v>
+        <v>22.4</v>
       </c>
       <c r="D17" s="2">
-        <v>20.18</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="E17" s="2">
-        <v>18.67</v>
+        <v>18.7</v>
       </c>
       <c r="F17" s="2">
-        <v>17.89</v>
+        <v>18.09</v>
       </c>
       <c r="G17" s="2">
-        <v>17.08</v>
+        <v>17.46</v>
       </c>
       <c r="H17" s="2">
-        <v>16.75</v>
+        <v>17.2</v>
       </c>
       <c r="I17" s="2">
-        <v>16.24</v>
+        <v>16.809999999999999</v>
       </c>
       <c r="J17" s="2">
-        <v>15.38</v>
+        <v>16.16</v>
       </c>
       <c r="K17" s="2">
-        <v>15.04</v>
+        <v>15.9</v>
       </c>
       <c r="L17" s="2">
-        <v>14.54</v>
+        <v>15.51</v>
       </c>
       <c r="M17" s="2">
-        <v>13.75</v>
+        <v>14.88</v>
       </c>
       <c r="N17" s="2">
-        <v>13.04</v>
+        <v>14.28</v>
       </c>
       <c r="O17" s="2">
-        <v>12.45</v>
+        <v>13.72</v>
       </c>
       <c r="P17" s="2">
-        <v>11.64</v>
+        <v>12.78</v>
       </c>
       <c r="Q17" s="2">
-        <v>11.38</v>
+        <v>12.13</v>
       </c>
       <c r="R17" s="2">
-        <v>11.68</v>
+        <v>11.78</v>
       </c>
       <c r="S17" s="2">
-        <v>15.44</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+        <v>12.77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>29.33</v>
+        <v>27.62</v>
       </c>
       <c r="C18" s="2">
-        <v>22.4</v>
+        <v>21.84</v>
       </c>
       <c r="D18" s="2">
-        <v>19.9</v>
+        <v>19.809999999999999</v>
       </c>
       <c r="E18" s="2">
-        <v>18.7</v>
+        <v>18.809999999999999</v>
       </c>
       <c r="F18" s="2">
-        <v>18.09</v>
+        <v>18.3</v>
       </c>
       <c r="G18" s="2">
-        <v>17.46</v>
+        <v>17.77</v>
       </c>
       <c r="H18" s="2">
-        <v>17.2</v>
+        <v>17.559999999999999</v>
       </c>
       <c r="I18" s="2">
-        <v>16.81</v>
+        <v>17.239999999999998</v>
       </c>
       <c r="J18" s="2">
+        <v>16.7</v>
+      </c>
+      <c r="K18" s="2">
+        <v>16.489999999999998</v>
+      </c>
+      <c r="L18" s="2">
         <v>16.16</v>
       </c>
-      <c r="K18" s="2">
-        <v>15.9</v>
-      </c>
-      <c r="L18" s="2">
-        <v>15.51</v>
-      </c>
       <c r="M18" s="2">
-        <v>14.88</v>
+        <v>15.63</v>
       </c>
       <c r="N18" s="2">
-        <v>14.28</v>
+        <v>15.11</v>
       </c>
       <c r="O18" s="2">
-        <v>13.72</v>
+        <v>14.61</v>
       </c>
       <c r="P18" s="2">
-        <v>12.78</v>
+        <v>13.71</v>
       </c>
       <c r="Q18" s="2">
-        <v>12.13</v>
+        <v>12.98</v>
       </c>
       <c r="R18" s="2">
-        <v>11.78</v>
+        <v>12.44</v>
       </c>
       <c r="S18" s="2">
-        <v>12.77</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+        <v>11.92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>27.62</v>
+        <v>25.74</v>
       </c>
       <c r="C19" s="2">
-        <v>21.84</v>
+        <v>21.49</v>
       </c>
       <c r="D19" s="2">
-        <v>19.81</v>
+        <v>19.95</v>
       </c>
       <c r="E19" s="2">
-        <v>18.81</v>
+        <v>19.21</v>
       </c>
       <c r="F19" s="2">
-        <v>18.3</v>
+        <v>18.82</v>
       </c>
       <c r="G19" s="2">
-        <v>17.77</v>
+        <v>18.43</v>
       </c>
       <c r="H19" s="2">
-        <v>17.56</v>
+        <v>18.27</v>
       </c>
       <c r="I19" s="2">
-        <v>17.24</v>
+        <v>18.03</v>
       </c>
       <c r="J19" s="2">
-        <v>16.7</v>
+        <v>17.63</v>
       </c>
       <c r="K19" s="2">
-        <v>16.49</v>
+        <v>17.46</v>
       </c>
       <c r="L19" s="2">
-        <v>16.16</v>
+        <v>17.22</v>
       </c>
       <c r="M19" s="2">
-        <v>15.63</v>
+        <v>16.8</v>
       </c>
       <c r="N19" s="2">
-        <v>15.11</v>
-      </c>
-      <c r="O19" s="2">
-        <v>14.61</v>
+        <v>16.399999999999999</v>
+      </c>
+      <c r="O19" s="3">
+        <v>16</v>
       </c>
       <c r="P19" s="2">
-        <v>13.71</v>
+        <v>15.25</v>
       </c>
       <c r="Q19" s="2">
-        <v>12.98</v>
+        <v>14.57</v>
       </c>
       <c r="R19" s="2">
-        <v>12.44</v>
+        <v>13.97</v>
       </c>
       <c r="S19" s="2">
-        <v>11.92</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2">
-        <v>25.74</v>
-      </c>
-      <c r="C20" s="2">
-        <v>21.49</v>
-      </c>
-      <c r="D20" s="2">
-        <v>19.95</v>
-      </c>
-      <c r="E20" s="2">
-        <v>19.21</v>
-      </c>
-      <c r="F20" s="2">
-        <v>18.82</v>
-      </c>
-      <c r="G20" s="2">
-        <v>18.43</v>
-      </c>
-      <c r="H20" s="2">
-        <v>18.27</v>
-      </c>
-      <c r="I20" s="2">
-        <v>18.03</v>
-      </c>
-      <c r="J20" s="2">
-        <v>17.63</v>
-      </c>
-      <c r="K20" s="2">
-        <v>17.46</v>
-      </c>
-      <c r="L20" s="2">
-        <v>17.22</v>
-      </c>
-      <c r="M20" s="2">
-        <v>16.8</v>
-      </c>
-      <c r="N20" s="2">
-        <v>16.4</v>
-      </c>
-      <c r="O20" s="3">
-        <v>16</v>
-      </c>
-      <c r="P20" s="2">
-        <v>15.25</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>14.57</v>
-      </c>
-      <c r="R20" s="2">
-        <v>13.97</v>
-      </c>
-      <c r="S20" s="2">
         <v>12.49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Debut nouvelle architecture, nouveau Euler Scheme &  abstact processes
</commit_message>
<xml_diff>
--- a/data/option_data/option_data_SPX.xlsx
+++ b/data/option_data/option_data_SPX.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thibc\OneDrive\Documents\Dev\Structured-Product-Pricing-Python\data\option_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://devinci-my.sharepoint.com/personal/jules_hellot_edu_devinci_fr/Documents/Dauphine A5/S2/Produits Structurés/Structured-Product-Pricing-Python/data/option_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F581E810-8FFA-46A7-9F8E-FD919AE204F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F581E810-8FFA-46A7-9F8E-FD919AE204F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3F973F7-863A-43F9-898B-E93C6A1409A9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -450,20 +450,20 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="14" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="14" width="7.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="7.88671875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +522,7 @@
         <v>8653.1</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -581,7 +581,7 @@
         <v>68.58</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -640,7 +640,7 @@
         <v>55.56</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -699,7 +699,7 @@
         <v>48.76</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -758,7 +758,7 @@
         <v>42.8</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -817,7 +817,7 @@
         <v>41.09</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -876,7 +876,7 @@
         <v>38.57</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -935,7 +935,7 @@
         <v>36.57</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -994,7 +994,7 @@
         <v>33.82</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>33.43</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>31.05</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>29.03</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>17.86</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>16.89</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>15.44</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>12.77</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>11.92</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>

</xml_diff>